<commit_message>
contains mac addresses of at least the 20 newest badges, just in case needed in the future
</commit_message>
<xml_diff>
--- a/module ids.xlsx
+++ b/module ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\badges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA4F313-C222-40A1-A2AE-3FEECCD50DB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7C51F1-90EF-46CE-B8E3-3375336E0C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Badge</t>
   </si>
@@ -51,20 +51,139 @@
     <t>b4:e6:2d:2d:54:16</t>
   </si>
   <si>
-    <t xml:space="preserve">
-b4:e6:2d:2d:54:1f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-b4:e6:2d:2d:54:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-b4:e6:2d:2d:54:73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-84:f3:eb:44:2e:c0</t>
+    <t>NEW BADGES</t>
+  </si>
+  <si>
+    <t>wx-19a16e</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:a1:6e</t>
+  </si>
+  <si>
+    <t>wx-a36ca3</t>
+  </si>
+  <si>
+    <t>84:f3:eb:a3:6c:a3</t>
+  </si>
+  <si>
+    <t>wx-2d5122</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:51:22</t>
+  </si>
+  <si>
+    <t>wx-19a16c</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:a1:6c</t>
+  </si>
+  <si>
+    <t>wx-2d512c</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:51:2c</t>
+  </si>
+  <si>
+    <t>wx-199e0d</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:9e:0d</t>
+  </si>
+  <si>
+    <t>wx-2d583a</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:58:3a</t>
+  </si>
+  <si>
+    <t>wx-a36bec</t>
+  </si>
+  <si>
+    <t>84:f3:eb:a3:6b:ec</t>
+  </si>
+  <si>
+    <t>wx-2d510c</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:51:0c</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:54:1f</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:54:26</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:54:73</t>
+  </si>
+  <si>
+    <t>84:f3:eb:44:2e:c0</t>
+  </si>
+  <si>
+    <t>wx-2d509d</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:50:9d</t>
+  </si>
+  <si>
+    <t>wx-2d4d75</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:4d:75</t>
+  </si>
+  <si>
+    <t>wx-19a12b</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:a1:2b</t>
+  </si>
+  <si>
+    <t>wx-a36d26</t>
+  </si>
+  <si>
+    <t>84:f3:eb:a3:6d:26</t>
+  </si>
+  <si>
+    <t>wx-199ee1</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:9e:e1</t>
+  </si>
+  <si>
+    <t>wx-2d5874</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:58:74</t>
+  </si>
+  <si>
+    <t>wx-199ee0</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:9e:e0</t>
+  </si>
+  <si>
+    <t>wx-19a164</t>
+  </si>
+  <si>
+    <t>ec:fa:bc:19:a1:64</t>
+  </si>
+  <si>
+    <t>wx-2d5852</t>
+  </si>
+  <si>
+    <t>b4:e6:2d:2d:58:52</t>
+  </si>
+  <si>
+    <t>wx-a36c30</t>
+  </si>
+  <si>
+    <t>84:f3:eb:a3:6c:30</t>
+  </si>
+  <si>
+    <t>wx-a36c28</t>
+  </si>
+  <si>
+    <t>84:f3:eb:a3:6c:28</t>
   </si>
 </sst>
 </file>
@@ -396,13 +515,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -412,12 +535,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -429,29 +552,194 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>